<commit_message>
Comparison Details first version done
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF4C47-8644-46B2-B44C-BBCB6B5F0DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0808B44-42AE-44BB-A1D1-FD1C5E2A4806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -183,7 +183,10 @@
     <t>WebApp</t>
   </si>
   <si>
-    <t>WebApp Comparision Overview</t>
+    <t>WebApp Comparison Overview</t>
+  </si>
+  <si>
+    <t>WebApp Comparison Detail</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +561,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -600,7 +603,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.18266666666666667</v>
+        <v>0.19333333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -993,6 +996,17 @@
       </c>
       <c r="C38" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45289</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tooltip for Classes and Path
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0808B44-42AE-44BB-A1D1-FD1C5E2A4806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE3CE37-8034-4627-A5A2-1D15044F18F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Datum</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>WebApp Comparison Detail</t>
+  </si>
+  <si>
+    <t>WebApp Graph/Version editable and deleteable</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +564,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -603,7 +606,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.19333333333333333</v>
+        <v>0.19733333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1007,6 +1010,17 @@
       </c>
       <c r="C39" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>45301</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
broken version of format text from model, todo fix utils
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D844076-FE88-4799-9DA4-23002E065576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1787D5EE-15A2-4BE4-8EA3-3B9826A59018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Datum</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Meeting + Proposal</t>
+  </si>
+  <si>
+    <t>Webapp comparison for detail view property shapes</t>
+  </si>
+  <si>
+    <t>Propsoal</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +579,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -615,7 +621,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.22266666666666668</v>
+        <v>0.22933333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -636,7 +642,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>6.68</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,6 +1120,28 @@
       </c>
       <c r="C47" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed blank node bug with jena pretty format, adapted formatting
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1787D5EE-15A2-4BE4-8EA3-3B9826A59018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A34D5-26C3-4522-B56E-80F639190D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Datum</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Propsoal</t>
+  </si>
+  <si>
+    <t>Bug Blank Nodes Anzeige</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +582,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -621,7 +624,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.22933333333333333</v>
+        <v>0.23333333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -642,7 +645,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>6.88</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1142,6 +1145,17 @@
       </c>
       <c r="C49" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search for overview implemented, filter not working yet
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A34D5-26C3-4522-B56E-80F639190D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA5436-CEEC-4F23-9BD2-4676337933EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>Datum</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Bug Blank Nodes Anzeige</t>
+  </si>
+  <si>
+    <t>Filter Overview</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +585,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -624,7 +627,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.23333333333333334</v>
+        <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -645,7 +648,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>7</v>
+        <v>7.32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1156,6 +1159,28 @@
       </c>
       <c r="C50" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>45357</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>45357</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter & Search finished
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA5436-CEEC-4F23-9BD2-4676337933EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED85360-548B-4E08-A065-40D95C31C4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Zeitplan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -211,6 +212,24 @@
   </si>
   <si>
     <t>Filter Overview</t>
+  </si>
+  <si>
+    <t>Stand Anfang März</t>
+  </si>
+  <si>
+    <t>Website fertig + why shapes were added Ende - März</t>
+  </si>
+  <si>
+    <t>für jeden Algorithmus 1 Monat + 1 Monat Spazi = Ende Juli</t>
+  </si>
+  <si>
+    <t>Alles auf VM, testen, Experimente 2 Monate - Ende September</t>
+  </si>
+  <si>
+    <t>Experteninterviews 1 Monat - Ende Oktober</t>
+  </si>
+  <si>
+    <t>Schreiben: 2 Monate Ende 2024</t>
   </si>
 </sst>
 </file>
@@ -539,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +604,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -627,7 +646,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.24399999999999999</v>
+        <v>0.24666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -648,7 +667,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>7.32</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1181,6 +1200,17 @@
       </c>
       <c r="C52" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>45358</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1190,15 +1220,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F2D98A-A4D8-4A9F-BF2C-1E834DE5242E}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45275</v>
       </c>
@@ -1214,7 +1244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44941</v>
       </c>
@@ -1222,7 +1252,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44986</v>
       </c>
@@ -1230,7 +1260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45000</v>
       </c>
@@ -1238,30 +1268,60 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugs fixed, e.g. Detailview: sort shacl shapes
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED85360-548B-4E08-A065-40D95C31C4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C6C23B-0925-422A-B755-45D4DFE63CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Datum</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Schreiben: 2 Monate Ende 2024</t>
+  </si>
+  <si>
+    <t>Navigation Session Variablen</t>
   </si>
 </sst>
 </file>
@@ -558,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +607,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -646,7 +649,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.24666666666666667</v>
+        <v>0.25066666666666665</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -667,7 +670,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>7.4</v>
+        <v>7.52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1211,6 +1214,17 @@
       </c>
       <c r="C53" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hierarchical colum, filter cached (not done yet)
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C6C23B-0925-422A-B755-45D4DFE63CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5DE2E0-ADCD-426F-9CDF-F2FB8166882F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Zeitplan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Datum</t>
   </si>
@@ -233,6 +232,15 @@
   </si>
   <si>
     <t>Navigation Session Variablen</t>
+  </si>
+  <si>
+    <t>Bugs fixen</t>
+  </si>
+  <si>
+    <t>Proposals Review</t>
+  </si>
+  <si>
+    <t>Ui fixes</t>
   </si>
 </sst>
 </file>
@@ -561,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +615,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -649,7 +657,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.25066666666666665</v>
+        <v>0.26266666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -670,7 +678,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>7.52</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1225,6 +1233,39 @@
       </c>
       <c r="C54" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>45364</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>45366</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugs & Info for deletion
Shactor/QSE Bugs resolved, why shapes were deleted added, default shapes added
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C48A577-F44B-4F95-869B-E5CE7B6FFF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33FEE79-B0B6-461B-8595-D097051437C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Meetings + VM</t>
+  </si>
+  <si>
+    <t>Presentation Vorb</t>
+  </si>
+  <si>
+    <t>Remove Supp and Conf, ShaclOrItems, Default Shapes saved</t>
   </si>
 </sst>
 </file>
@@ -572,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +624,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -660,7 +666,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.26666666666666666</v>
+        <v>0.27466666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -681,7 +687,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>8</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1291,6 +1297,28 @@
       </c>
       <c r="C59" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplify graph upload (not tested)
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96C260-4570-4042-B528-4AC570FC096A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD81E1-2777-4086-B21D-8C020E4D2D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Datum</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Proposal Presentation</t>
+  </si>
+  <si>
+    <t>VM einrichten, WebApp testen mit echten Daten</t>
   </si>
 </sst>
 </file>
@@ -584,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +633,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,7 +675,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.29199999999999998</v>
+        <v>0.30266666666666664</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -693,7 +696,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>8.76</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1347,6 +1350,17 @@
       </c>
       <c r="C63" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started to save shapes as file
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD81E1-2777-4086-B21D-8C020E4D2D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D22837-9023-4CD2-886F-444D85D9EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>Datum</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>VM einrichten, WebApp testen mit echten Daten</t>
+  </si>
+  <si>
+    <t>Load pre-configured graphs, performance problems</t>
   </si>
 </sst>
 </file>
@@ -587,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,7 +636,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -675,7 +678,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.30266666666666664</v>
+        <v>0.31333333333333335</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -696,7 +699,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>9.08</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1361,6 +1364,17 @@
       </c>
       <c r="C64" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>45379</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug generate text when shape is not included anyways
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D0D1D9-3A9D-4D9A-BF43-96DC28247EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E1C157-0AA7-493D-8647-3F9B0EF25011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>Datum</t>
   </si>
@@ -593,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.31733333333333336</v>
+        <v>0.32666666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -702,7 +702,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>9.52</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1388,6 +1388,17 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>45384</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
handling large strings in diff (not done)
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C59D8BC-5089-4126-9733-9CA5226E9C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3E337F-BC20-4B7E-85DF-CFDBCC3E63B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.33200000000000002</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -702,7 +702,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>9.9600000000000009</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1407,7 +1407,7 @@
         <v>45385</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Fixed Or Items Order Bug
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DCE8B7-E277-4483-B89C-6EFFC2A1A724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FFD056-1A4E-454D-9486-C6B70159BC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>Datum</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Planen, Bugfixes</t>
+  </si>
+  <si>
+    <t>Bugfixes</t>
   </si>
 </sst>
 </file>
@@ -599,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +648,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -687,7 +690,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.34</v>
+        <v>0.34666666666666668</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,7 +711,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>10.199999999999999</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1450,6 +1453,17 @@
       </c>
       <c r="C71" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>45391</v>
+      </c>
+      <c r="B72">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get db creation script
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FFD056-1A4E-454D-9486-C6B70159BC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68704389-5800-4D6B-B099-F541A218C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Datum</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Bugfixes</t>
+  </si>
+  <si>
+    <t>Schreiben</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +651,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -690,7 +693,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.34666666666666668</v>
+        <v>0.35466666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -711,7 +714,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>10.4</v>
+        <v>10.64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1464,6 +1467,28 @@
       </c>
       <c r="C72" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>45394</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>45394</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started RQ4, QSE adapted from main
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68704389-5800-4D6B-B099-F541A218C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CCB5C9-CDAF-4E42-9A53-E1B5C18DB3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Datum</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Schreiben</t>
+  </si>
+  <si>
+    <t>RQ1 schreiben</t>
+  </si>
+  <si>
+    <t>QSE für Query Based probieren</t>
   </si>
 </sst>
 </file>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +657,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -693,7 +699,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.35466666666666669</v>
+        <v>0.36399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -714,7 +720,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>10.64</v>
+        <v>10.92</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1489,6 +1495,28 @@
       </c>
       <c r="C74" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>45399</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>45399</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started with RQ4, QSE QueryBased not working
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CCB5C9-CDAF-4E42-9A53-E1B5C18DB3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637F4CFC-491C-4498-8FBF-8B43FEE1E244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>Datum</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>QSE für Query Based probieren</t>
+  </si>
+  <si>
+    <t>RQ4 anfangen -&gt; QSE QB geht nicht</t>
   </si>
 </sst>
 </file>
@@ -611,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,7 +660,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -699,7 +702,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.36399999999999999</v>
+        <v>0.37466666666666665</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -720,7 +723,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>10.92</v>
+        <v>11.24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1517,6 +1520,17 @@
       </c>
       <c r="C76" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>45401</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QSE now on current status
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637F4CFC-491C-4498-8FBF-8B43FEE1E244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CA5660-ADEF-4B87-8847-552764FF21D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>Datum</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>RQ4 anfangen -&gt; QSE QB geht nicht</t>
+  </si>
+  <si>
+    <t>QSE Bugfixes bei QueryBased, Vergleiche zwischen QB und FB</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +663,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -702,7 +705,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.37466666666666665</v>
+        <v>0.38266666666666665</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -723,7 +726,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>11.24</v>
+        <v>11.48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1531,6 +1534,17 @@
       </c>
       <c r="C77" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B78">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RQ4 basic propertyshapes work
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE334766-B5F6-40D0-B848-E647A01AA122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D09AA5-A9D0-4F50-8116-03A0B3C2E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>Datum</t>
   </si>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,7 +708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.39333333333333331</v>
+        <v>0.39733333333333332</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>11.8</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1569,6 +1569,17 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RQ4, began with or list items
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D09AA5-A9D0-4F50-8116-03A0B3C2E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B058B2B-C5DA-488F-9A55-073AA2C0BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,7 +708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.39733333333333332</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>11.92</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1577,7 +1577,7 @@
         <v>45415</v>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Started implementing or items
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B058B2B-C5DA-488F-9A55-073AA2C0BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2DB1E-7B29-4EAB-8836-E2DEEC8CB75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
   <si>
     <t>Datum</t>
   </si>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,7 +708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.4</v>
+        <v>0.40133333333333332</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>12</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1580,6 +1580,17 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refined or list items, added tests for deletion (not finished)
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2DB1E-7B29-4EAB-8836-E2DEEC8CB75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B674FA-97C8-4138-9317-1C26FEB56A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Datum</t>
   </si>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,7 +708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.40133333333333332</v>
+        <v>0.40933333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>12.04</v>
+        <v>12.28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1591,6 +1591,17 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B83">
+        <v>6</v>
+      </c>
+      <c r="C83" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1603,7 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F2D98A-A4D8-4A9F-BF2C-1E834DE5242E}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Started using objects in RQ4 based on Shactor QSE (not working)
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E118082B-E933-4DF2-B1D0-BF199CB87A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F88AA7-E71D-40F0-B285-D58714BC31AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>Datum</t>
   </si>
@@ -653,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,7 +699,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -741,7 +741,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.47066666666666668</v>
+        <v>0.47333333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>14.12</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1838,12 +1838,23 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>45446</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continued in leave only one or item
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498072AD-98C1-49EF-A560-85A139D2D518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFECD81-53B3-4CFA-959E-8E31F9BF5166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>Datum</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Geschriebenes kontrollieren</t>
+  </si>
+  <si>
+    <t>RQ4 - or item ein item left, weiterschreiben</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +705,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -744,7 +747,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.48266666666666669</v>
+        <v>0.48666666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -765,7 +768,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>14.48</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1888,10 +1891,21 @@
         <v>45447</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C106" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>45448</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of two QSE comparison runs
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFECD81-53B3-4CFA-959E-8E31F9BF5166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ED09A1-9E17-49B4-B6AA-78E903AAE476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
   <si>
     <t>Datum</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>RQ4 - or item ein item left, weiterschreiben</t>
+  </si>
+  <si>
+    <t>RQ4 - Comparison between two QSE runs</t>
   </si>
 </sst>
 </file>
@@ -394,6 +397,1510 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stunden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$107</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="106"/>
+                <c:pt idx="0">
+                  <c:v>45146</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45147</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45177</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45189</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45208</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45209</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45212</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45214</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45215</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45219</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45234</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45236</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45239</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45243</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45244</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45245</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45253</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45254</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45257</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45258</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45259</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45260</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45264</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45273</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>45274</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45275</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45280</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45282</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45287</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45288</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>45289</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>45299</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45301</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45315</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45316</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45320</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45322</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45324</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45353</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45356</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>45356</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>45356</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45357</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45357</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45358</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>45359</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>45359</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>45364</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>45366</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>45368</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>45370</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>45370</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>45371</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>45373</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>45377</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>45379</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>45380</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>45384</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45385</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>45387</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>45387</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>45391</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45391</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>45394</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>45394</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>45399</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>45399</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>45401</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>45405</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>45406</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>45412</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>45415</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>45416</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>45419</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>45420</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>45420</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>45422</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>45423</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>45426</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>45426</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>45427</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>45429</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>45429</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>45432</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>45432</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>45434</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>45436</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>45437</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>45438</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>45439</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>45439</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>45441</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>45441</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>45446</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>45447</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>45447</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>45447</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>45448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$2:$B$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="106"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-29F3-43D6-A3D9-1A4F7F0FF13E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="25977648"/>
+        <c:axId val="25984848"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="25977648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="25984848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="25984848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="25977648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>177165</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>481965</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50482</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEECF20F-D6EA-6278-3254-43CC927C251B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -659,10 +2166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,7 +2212,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -747,7 +2254,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.48666666666666669</v>
+        <v>0.49066666666666664</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -768,7 +2275,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>14.6</v>
+        <v>14.72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1908,8 +3415,20 @@
         <v>97</v>
       </c>
     </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>45449</v>
+      </c>
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="C108" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed Paths for VM
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E23DC-479F-4E15-95E0-328349CEB7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A54F791-603B-4E8B-90A6-B2531F48DF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
   <si>
     <t>Datum</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Soll</t>
+  </si>
+  <si>
+    <t>minus</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -439,7 +442,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2103,7 +2105,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CF8BE12-5E12-4E39-A988-EAD0A6A77ED9}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CF8BE12-5E12-4E39-A988-EAD0A6A77ED9}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="G8:H20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" numFmtId="16" showAll="0">
@@ -2580,10 +2582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,7 +2600,7 @@
     <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45146</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45147</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45162</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>0.5053333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45177</v>
       </c>
@@ -2696,7 +2698,7 @@
         <v>15.16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45178</v>
       </c>
@@ -2710,7 +2712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45184</v>
       </c>
@@ -2724,7 +2726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45189</v>
       </c>
@@ -2746,8 +2748,11 @@
       <c r="I8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45202</v>
       </c>
@@ -2763,14 +2768,18 @@
       <c r="G9" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <v>15</v>
       </c>
       <c r="I9">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f>(I9-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",1))*-1</f>
+        <v>-48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45204</v>
       </c>
@@ -2786,14 +2795,18 @@
       <c r="G10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <v>3</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f>(I10-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",2))*-1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45208</v>
       </c>
@@ -2806,14 +2819,18 @@
       <c r="G11" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11">
         <v>75</v>
       </c>
       <c r="I11">
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f>(I11-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",3))*-1</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45209</v>
       </c>
@@ -2826,14 +2843,18 @@
       <c r="G12" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <v>57</v>
       </c>
       <c r="I12">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f>(I12-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",4))*-1</f>
+        <v>-68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45210</v>
       </c>
@@ -2846,14 +2867,18 @@
       <c r="G13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13">
         <v>58</v>
       </c>
       <c r="I13">
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <f>(I13-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",5))*-1</f>
+        <v>-67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45212</v>
       </c>
@@ -2866,14 +2891,18 @@
       <c r="G14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <v>26</v>
       </c>
       <c r="I14">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f>(I14-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",6))*-1</f>
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45214</v>
       </c>
@@ -2886,14 +2915,18 @@
       <c r="G15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15">
         <v>6</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <f>(I15-0)*-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45215</v>
       </c>
@@ -2906,14 +2939,18 @@
       <c r="G16" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16">
         <v>18</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <f>(I16-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",9))*-1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45219</v>
       </c>
@@ -2926,14 +2963,18 @@
       <c r="G17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17">
         <v>33</v>
       </c>
       <c r="I17">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <f>(I17-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",10))*-1</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45234</v>
       </c>
@@ -2946,14 +2987,18 @@
       <c r="G18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18">
         <v>48</v>
       </c>
       <c r="I18">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f>(I18-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",11))*-1</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45236</v>
       </c>
@@ -2966,14 +3011,18 @@
       <c r="G19" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19">
         <v>40</v>
       </c>
       <c r="I19">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f>(I19-GETPIVOTDATA("Stunden",$G$8,"Months (Datum)",12))*-1</f>
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45239</v>
       </c>
@@ -2986,11 +3035,11 @@
       <c r="G20" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20">
         <v>379</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45240</v>
       </c>
@@ -3001,7 +3050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45243</v>
       </c>
@@ -3012,7 +3061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45244</v>
       </c>
@@ -3023,7 +3072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45245</v>
       </c>
@@ -3034,7 +3083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45253</v>
       </c>
@@ -3045,7 +3094,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45254</v>
       </c>
@@ -3056,7 +3105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45257</v>
       </c>
@@ -3067,7 +3116,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45258</v>
       </c>
@@ -3078,7 +3127,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45259</v>
       </c>
@@ -3089,7 +3138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45260</v>
       </c>
@@ -3100,7 +3149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45264</v>
       </c>
@@ -3111,7 +3160,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45273</v>
       </c>

</xml_diff>

<commit_message>
Bugfix RQ4, delete node shape when there are no further propertyshapes
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5F451F-2169-471F-A95F-29FF86FA6D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6424D84A-28EE-4062-8CCB-1C36A39BA152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="125">
   <si>
     <t>Datum</t>
   </si>
@@ -2615,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2665,7 +2666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>448</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2707,7 +2708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.59733333333333338</v>
+        <v>0.60666666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2728,7 +2729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>17.920000000000002</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4246,6 +4247,28 @@
         <v>3</v>
       </c>
       <c r="C127" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>45473</v>
+      </c>
+      <c r="B128" s="6">
+        <v>5</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>45474</v>
+      </c>
+      <c r="B129" s="6">
+        <v>2</v>
+      </c>
+      <c r="C129" s="6" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert changes from yesterday
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6424D84A-28EE-4062-8CCB-1C36A39BA152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4370DD7E-608B-4AB3-BE1A-BAD74AD80F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
   <si>
     <t>Datum</t>
   </si>
@@ -2616,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2666,7 +2666,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>455</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.60666666666666669</v>
+        <v>0.61466666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>18.2</v>
+        <v>18.440000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4269,6 +4269,17 @@
         <v>2</v>
       </c>
       <c r="C129" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>45475</v>
+      </c>
+      <c r="B130" s="6">
+        <v>6</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logic for added shapes
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08285C4C-49F8-4EC0-8FD0-C479E91C2A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52490F1-CEA9-46AA-80FD-FDB440A83FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="127">
   <si>
     <t>Datum</t>
   </si>
@@ -2621,10 +2621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="C136" activeCellId="1" sqref="D135 C136"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>484</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.64533333333333331</v>
+        <v>0.66133333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>19.36</v>
+        <v>19.84</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4340,6 +4340,28 @@
         <v>5</v>
       </c>
       <c r="C135" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>45490</v>
+      </c>
+      <c r="B136" s="6">
+        <v>6</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>45492</v>
+      </c>
+      <c r="B137" s="6">
+        <v>6</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ERD updated in RQ1, writing updates
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5507368-0950-411D-A085-373D418E7EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0512311E-61E8-4B4C-A160-89995FD12859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="129">
   <si>
     <t>Datum</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>RQ2</t>
+  </si>
+  <si>
+    <t>RQ2, Feedback einarbeiten</t>
+  </si>
+  <si>
+    <t>Feedback einarbeiten</t>
   </si>
 </sst>
 </file>
@@ -2621,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J139"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,7 +2677,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>506</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2713,7 +2719,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.67466666666666664</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2734,7 +2740,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>20.239999999999998</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4384,7 +4390,51 @@
         <v>7</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
+        <v>45497</v>
+      </c>
+      <c r="B140" s="6">
+        <v>8</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="1">
+        <v>45499</v>
+      </c>
+      <c r="B141" s="6">
+        <v>4</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="1">
+        <v>45501</v>
+      </c>
+      <c r="B142" s="6">
+        <v>1</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="1">
+        <v>45503</v>
+      </c>
+      <c r="B143" s="6">
+        <v>6</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Visual adjustments WebApp comparison detail view
</commit_message>
<xml_diff>
--- a/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
+++ b/QseEvolvingKgWebApp/notes/Aufwand_git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evapu\Documents\GitHub\QseEvolvingKg\QseEvolvingKgWebApp\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0512311E-61E8-4B4C-A160-89995FD12859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C4CB80-14D6-4C8A-BFD3-AE331BAC59CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="130">
   <si>
     <t>Datum</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Feedback einarbeiten</t>
+  </si>
+  <si>
+    <t>Meeting, Feedback einarbeiten</t>
   </si>
 </sst>
 </file>
@@ -2627,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,7 +2680,7 @@
       </c>
       <c r="G2">
         <f>SUM(B:B)</f>
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2719,7 +2722,7 @@
       </c>
       <c r="G4" s="2">
         <f>G2/G3</f>
-        <v>0.7</v>
+        <v>0.70399999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2740,7 +2743,7 @@
       </c>
       <c r="G5">
         <f>G2/25</f>
-        <v>21</v>
+        <v>21.12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4435,6 +4438,17 @@
       </c>
       <c r="C143" s="6" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="1">
+        <v>45504</v>
+      </c>
+      <c r="B144" s="6">
+        <v>3</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>